<commit_message>
adc scaling corrected to proper ax+b version. Excel calculator for a and parameters added
</commit_message>
<xml_diff>
--- a/Winch Controller/Winch Controller Object Dictionary.xlsx
+++ b/Winch Controller/Winch Controller Object Dictionary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="68">
   <si>
     <t>Index</t>
   </si>
@@ -203,12 +203,6 @@
     <t>Board position</t>
   </si>
   <si>
-    <t>ADC board position max</t>
-  </si>
-  <si>
-    <t>ADC board position min</t>
-  </si>
-  <si>
     <t>raw value when board is up</t>
   </si>
   <si>
@@ -216,6 +210,21 @@
   </si>
   <si>
     <t>S16</t>
+  </si>
+  <si>
+    <t>ADC board position offset</t>
+  </si>
+  <si>
+    <t>ADC board position scale</t>
+  </si>
+  <si>
+    <t>Board position max value</t>
+  </si>
+  <si>
+    <t>Board position min value</t>
+  </si>
+  <si>
+    <t>final value</t>
   </si>
 </sst>
 </file>
@@ -294,15 +303,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -588,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K25"/>
+  <dimension ref="B2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -603,7 +616,7 @@
     <col min="6" max="10" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:10">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -632,11 +645,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:11">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="2:10">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
@@ -658,9 +671,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:11">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+    <row r="4" spans="2:10">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
       <c r="D4" t="s">
         <v>15</v>
       </c>
@@ -680,9 +693,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+    <row r="5" spans="2:10">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
       <c r="D5" t="s">
         <v>17</v>
       </c>
@@ -702,21 +715,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="2:10">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
         <v>20</v>
@@ -728,20 +741,20 @@
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
@@ -753,75 +766,68 @@
         <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" s="4" customFormat="1">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" s="4" customFormat="1">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G10" t="s">
         <v>20</v>
@@ -832,15 +838,18 @@
       <c r="I10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="2:11">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
@@ -855,112 +864,116 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:11">
-      <c r="B12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
+    <row r="12" spans="2:10">
+      <c r="B12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="G12" t="s">
         <v>20</v>
       </c>
       <c r="H12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11">
-      <c r="B13" s="6"/>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>
       </c>
       <c r="H13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11">
-      <c r="B14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>39</v>
+      <c r="E14" t="s">
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
         <v>20</v>
       </c>
       <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11">
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="7"/>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>41</v>
+      <c r="E15" t="s">
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s">
         <v>20</v>
       </c>
       <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11">
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
@@ -974,16 +987,15 @@
       <c r="I16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -998,62 +1010,63 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="2:11">
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9">
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="F20" t="s">
         <v>33</v>
@@ -1068,14 +1081,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
+    <row r="21" spans="2:11">
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
         <v>33</v>
@@ -1090,62 +1103,62 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="2:11">
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C24" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9">
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9">
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
@@ -1160,14 +1173,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
+    <row r="25" spans="2:11">
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>
@@ -1182,23 +1195,67 @@
         <v>40</v>
       </c>
     </row>
+    <row r="26" spans="2:11">
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>
   <headerFooter>

</xml_diff>